<commit_message>
Added remaining numerical functions
</commit_message>
<xml_diff>
--- a/Numerical Functions in Excel.xlsx
+++ b/Numerical Functions in Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitb\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Learning Data analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8D7C67-7190-4CF1-B934-7EC62832C9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D82928A-B65B-458D-91D8-DC3A3DAC6126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{185D97FB-E57A-40AF-8DED-82FB167AC6E9}"/>
   </bookViews>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62969727-D2CB-4E5C-8B05-B5B7B716F001}">
   <dimension ref="A1:Q1471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="G1454" workbookViewId="0">
+      <selection activeCell="P1472" sqref="P1472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1305,7 +1305,9 @@
       <c r="M18">
         <v>0</v>
       </c>
-      <c r="P18" s="3"/>
+      <c r="P18" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="Q18" s="1"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
@@ -1332,9 +1334,6 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H19" t="s">
-        <v>37</v>
-      </c>
       <c r="I19">
         <v>7</v>
       </c>
@@ -1349,6 +1348,10 @@
       </c>
       <c r="M19">
         <v>0</v>
+      </c>
+      <c r="P19">
+        <f>COUNTIFS(M2:M1471, "0",L2:L1471,"3")</f>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
@@ -1375,10 +1378,6 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="H20" t="e">
-        <f>COUNTIFS(G2:G1471,G1077,I1:I1471,I1075)</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="I20">
         <v>1</v>
       </c>
@@ -56970,14 +56969,14 @@
         <v>11</v>
       </c>
       <c r="E1410" t="str">
-        <f t="shared" ref="E1410:E1473" si="44">UPPER(CONCATENATE(LEFT(D1410,3),A1410,LEFT(B1410,1)))</f>
+        <f t="shared" ref="E1410:E1471" si="44">UPPER(CONCATENATE(LEFT(D1410,3),A1410,LEFT(B1410,1)))</f>
         <v>SAL1613M</v>
       </c>
       <c r="F1410">
         <v>1</v>
       </c>
       <c r="G1410">
-        <f t="shared" ref="G1410:G1473" si="45">F1410*$P$2</f>
+        <f t="shared" ref="G1410:G1471" si="45">F1410*$P$2</f>
         <v>2.5</v>
       </c>
       <c r="I1410">

</xml_diff>